<commit_message>
Started working on Kiyosaki post
</commit_message>
<xml_diff>
--- a/data/snp500.xlsx
+++ b/data/snp500.xlsx
@@ -8,15 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/malshe/Dropbox/Work/R/dataviz-blog/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{F1C8D198-A551-C649-8E63-665D5A2308A6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{75E811AB-56E5-8940-BB12-3DFBEBB45707}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="380" yWindow="0" windowWidth="28040" windowHeight="16960" xr2:uid="{04CA6C6C-17A2-F049-A7CB-0C82B6C2CF74}"/>
+    <workbookView xWindow="380" yWindow="0" windowWidth="28040" windowHeight="16960" activeTab="2" xr2:uid="{04CA6C6C-17A2-F049-A7CB-0C82B6C2CF74}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -35,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="47">
   <si>
     <t>Date</t>
   </si>
@@ -60,15 +61,132 @@
   <si>
     <t>Returns</t>
   </si>
+  <si>
+    <t>twitter-2020-03-21</t>
+  </si>
+  <si>
+    <t>twitter-2020-03-23</t>
+  </si>
+  <si>
+    <t>twitter-2020-04-17</t>
+  </si>
+  <si>
+    <t>twitter-2020-07-20</t>
+  </si>
+  <si>
+    <t>twitter-2020-07-31</t>
+  </si>
+  <si>
+    <t>twitter-2020-08-13</t>
+  </si>
+  <si>
+    <t>twitter-2020-09-25</t>
+  </si>
+  <si>
+    <t>twitter-2020-10-02</t>
+  </si>
+  <si>
+    <t>twitter-2020-10-06</t>
+  </si>
+  <si>
+    <t>twitter-2020-10-28</t>
+  </si>
+  <si>
+    <t>twitter-2021-04-10</t>
+  </si>
+  <si>
+    <t>twitter-2021-04-16</t>
+  </si>
+  <si>
+    <t>twitter-2021-05-16</t>
+  </si>
+  <si>
+    <t>twitter-2021-06-18</t>
+  </si>
+  <si>
+    <t>twitter-2021-06-27</t>
+  </si>
+  <si>
+    <t>twitter-2021-07-31</t>
+  </si>
+  <si>
+    <t>twitter-2021-09-22</t>
+  </si>
+  <si>
+    <t>twitter-2021-09-23</t>
+  </si>
+  <si>
+    <t>twitter-2021-09-26</t>
+  </si>
+  <si>
+    <t>tweet_url</t>
+  </si>
+  <si>
+    <t>https://raw.githubusercontent.com/ashgreat/dataviz-blog/main/Images/therealkiyosaki/twitter-2020-03-21.png</t>
+  </si>
+  <si>
+    <t>https://raw.githubusercontent.com/ashgreat/dataviz-blog/main/Images/therealkiyosaki/twitter-2020-03-23.png</t>
+  </si>
+  <si>
+    <t>https://raw.githubusercontent.com/ashgreat/dataviz-blog/main/Images/therealkiyosaki/twitter-2020-04-17.png</t>
+  </si>
+  <si>
+    <t>https://raw.githubusercontent.com/ashgreat/dataviz-blog/main/Images/therealkiyosaki/twitter-2020-07-20.png</t>
+  </si>
+  <si>
+    <t>https://raw.githubusercontent.com/ashgreat/dataviz-blog/main/Images/therealkiyosaki/twitter-2020-07-31.png</t>
+  </si>
+  <si>
+    <t>https://raw.githubusercontent.com/ashgreat/dataviz-blog/main/Images/therealkiyosaki/twitter-2020-08-13.png</t>
+  </si>
+  <si>
+    <t>https://raw.githubusercontent.com/ashgreat/dataviz-blog/main/Images/therealkiyosaki/twitter-2020-09-25.png</t>
+  </si>
+  <si>
+    <t>https://raw.githubusercontent.com/ashgreat/dataviz-blog/main/Images/therealkiyosaki/twitter-2020-10-02.png</t>
+  </si>
+  <si>
+    <t>https://raw.githubusercontent.com/ashgreat/dataviz-blog/main/Images/therealkiyosaki/twitter-2020-10-06.png</t>
+  </si>
+  <si>
+    <t>https://raw.githubusercontent.com/ashgreat/dataviz-blog/main/Images/therealkiyosaki/twitter-2020-10-28.png</t>
+  </si>
+  <si>
+    <t>https://raw.githubusercontent.com/ashgreat/dataviz-blog/main/Images/therealkiyosaki/twitter-2021-04-10.png</t>
+  </si>
+  <si>
+    <t>https://raw.githubusercontent.com/ashgreat/dataviz-blog/main/Images/therealkiyosaki/twitter-2021-04-16.png</t>
+  </si>
+  <si>
+    <t>https://raw.githubusercontent.com/ashgreat/dataviz-blog/main/Images/therealkiyosaki/twitter-2021-05-16.png</t>
+  </si>
+  <si>
+    <t>https://raw.githubusercontent.com/ashgreat/dataviz-blog/main/Images/therealkiyosaki/twitter-2021-06-18.png</t>
+  </si>
+  <si>
+    <t>https://raw.githubusercontent.com/ashgreat/dataviz-blog/main/Images/therealkiyosaki/twitter-2021-06-27.png</t>
+  </si>
+  <si>
+    <t>https://raw.githubusercontent.com/ashgreat/dataviz-blog/main/Images/therealkiyosaki/twitter-2021-07-31.png</t>
+  </si>
+  <si>
+    <t>https://raw.githubusercontent.com/ashgreat/dataviz-blog/main/Images/therealkiyosaki/twitter-2021-09-22.png</t>
+  </si>
+  <si>
+    <t>https://raw.githubusercontent.com/ashgreat/dataviz-blog/main/Images/therealkiyosaki/twitter-2021-09-23.png</t>
+  </si>
+  <si>
+    <t>https://raw.githubusercontent.com/ashgreat/dataviz-blog/main/Images/therealkiyosaki/twitter-2021-09-26.png</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="169" formatCode="0.000%"/>
+    <numFmt numFmtId="164" formatCode="0.000%"/>
   </numFmts>
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -101,6 +219,14 @@
       <name val="Helvetica Neue"/>
       <family val="2"/>
     </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -119,11 +245,12 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="15" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -133,9 +260,11 @@
     <xf numFmtId="4" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="4" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="3" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="2"/>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="3">
+    <cellStyle name="Hyperlink" xfId="2" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Percent" xfId="1" builtinId="5"/>
   </cellStyles>
@@ -451,8 +580,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{32EEA70E-CF49-7F46-8EEC-1830E9F2E878}">
   <dimension ref="A1:H399"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H5" sqref="H5"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -10905,7 +11034,7 @@
         <v>8755780000</v>
       </c>
       <c r="H387" s="9">
-        <f t="shared" ref="H387:H399" si="6">(F387-F388)/F388</f>
+        <f t="shared" ref="H387:H398" si="6">(F387-F388)/F388</f>
         <v>-5.1830823307066745E-2</v>
       </c>
     </row>
@@ -11238,19 +11367,21 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{99A31F08-3525-4E44-8A96-0B0839BF79A8}">
-  <dimension ref="A1:C19"/>
+  <dimension ref="A1:E21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
+      <selection activeCell="E19" sqref="E1:E19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="17" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="11.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="17" bestFit="1" customWidth="1"/>
+    <col min="5" max="6" width="86.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A1" s="3">
         <v>43911</v>
       </c>
@@ -11261,8 +11392,15 @@
       <c r="C1" s="2">
         <v>43910</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="D1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E1" t="str">
+        <f>"https://raw.githubusercontent.com/ashgreat/dataviz-blog/main/Images/therealkiyosaki/"&amp;D1&amp;".png"</f>
+        <v>https://raw.githubusercontent.com/ashgreat/dataviz-blog/main/Images/therealkiyosaki/twitter-2020-03-21.png</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A2" s="3">
         <v>43913</v>
       </c>
@@ -11273,8 +11411,15 @@
       <c r="C2" s="3">
         <v>43913</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="D2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E2" t="str">
+        <f t="shared" ref="E2:E19" si="0">"https://raw.githubusercontent.com/ashgreat/dataviz-blog/main/Images/therealkiyosaki/"&amp;D2&amp;".png"</f>
+        <v>https://raw.githubusercontent.com/ashgreat/dataviz-blog/main/Images/therealkiyosaki/twitter-2020-03-23.png</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A3" s="3">
         <v>43938</v>
       </c>
@@ -11285,8 +11430,15 @@
       <c r="C3" s="3">
         <v>43938</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="D3" t="s">
+        <v>10</v>
+      </c>
+      <c r="E3" t="str">
+        <f t="shared" si="0"/>
+        <v>https://raw.githubusercontent.com/ashgreat/dataviz-blog/main/Images/therealkiyosaki/twitter-2020-04-17.png</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A4" s="3">
         <v>44032</v>
       </c>
@@ -11297,8 +11449,15 @@
       <c r="C4" s="3">
         <v>44032</v>
       </c>
-    </row>
-    <row r="5" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="D4" t="s">
+        <v>11</v>
+      </c>
+      <c r="E4" t="str">
+        <f t="shared" si="0"/>
+        <v>https://raw.githubusercontent.com/ashgreat/dataviz-blog/main/Images/therealkiyosaki/twitter-2020-07-20.png</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A5" s="3">
         <v>44043</v>
       </c>
@@ -11309,8 +11468,15 @@
       <c r="C5" s="3">
         <v>44043</v>
       </c>
-    </row>
-    <row r="6" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="D5" t="s">
+        <v>12</v>
+      </c>
+      <c r="E5" t="str">
+        <f t="shared" si="0"/>
+        <v>https://raw.githubusercontent.com/ashgreat/dataviz-blog/main/Images/therealkiyosaki/twitter-2020-07-31.png</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A6" s="3">
         <v>44056</v>
       </c>
@@ -11321,8 +11487,15 @@
       <c r="C6" s="3">
         <v>44056</v>
       </c>
-    </row>
-    <row r="7" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="D6" t="s">
+        <v>13</v>
+      </c>
+      <c r="E6" t="str">
+        <f t="shared" si="0"/>
+        <v>https://raw.githubusercontent.com/ashgreat/dataviz-blog/main/Images/therealkiyosaki/twitter-2020-08-13.png</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A7" s="3">
         <v>44099</v>
       </c>
@@ -11333,8 +11506,15 @@
       <c r="C7" s="3">
         <v>44099</v>
       </c>
-    </row>
-    <row r="8" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="D7" t="s">
+        <v>14</v>
+      </c>
+      <c r="E7" t="str">
+        <f t="shared" si="0"/>
+        <v>https://raw.githubusercontent.com/ashgreat/dataviz-blog/main/Images/therealkiyosaki/twitter-2020-09-25.png</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A8" s="3">
         <v>44106</v>
       </c>
@@ -11345,8 +11525,15 @@
       <c r="C8" s="3">
         <v>44106</v>
       </c>
-    </row>
-    <row r="9" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="D8" t="s">
+        <v>15</v>
+      </c>
+      <c r="E8" t="str">
+        <f t="shared" si="0"/>
+        <v>https://raw.githubusercontent.com/ashgreat/dataviz-blog/main/Images/therealkiyosaki/twitter-2020-10-02.png</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A9" s="3">
         <v>44110</v>
       </c>
@@ -11357,8 +11544,15 @@
       <c r="C9" s="3">
         <v>44110</v>
       </c>
-    </row>
-    <row r="10" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="D9" t="s">
+        <v>16</v>
+      </c>
+      <c r="E9" t="str">
+        <f t="shared" si="0"/>
+        <v>https://raw.githubusercontent.com/ashgreat/dataviz-blog/main/Images/therealkiyosaki/twitter-2020-10-06.png</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A10" s="3">
         <v>44132</v>
       </c>
@@ -11369,8 +11563,15 @@
       <c r="C10" s="3">
         <v>44132</v>
       </c>
-    </row>
-    <row r="11" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="D10" t="s">
+        <v>17</v>
+      </c>
+      <c r="E10" t="str">
+        <f t="shared" si="0"/>
+        <v>https://raw.githubusercontent.com/ashgreat/dataviz-blog/main/Images/therealkiyosaki/twitter-2020-10-28.png</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A11" s="3">
         <v>44296</v>
       </c>
@@ -11381,8 +11582,15 @@
       <c r="C11" s="2">
         <v>44295</v>
       </c>
-    </row>
-    <row r="12" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="D11" t="s">
+        <v>18</v>
+      </c>
+      <c r="E11" t="str">
+        <f t="shared" si="0"/>
+        <v>https://raw.githubusercontent.com/ashgreat/dataviz-blog/main/Images/therealkiyosaki/twitter-2021-04-10.png</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A12" s="3">
         <v>44302</v>
       </c>
@@ -11393,8 +11601,15 @@
       <c r="C12" s="3">
         <v>44302</v>
       </c>
-    </row>
-    <row r="13" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="D12" t="s">
+        <v>19</v>
+      </c>
+      <c r="E12" t="str">
+        <f t="shared" si="0"/>
+        <v>https://raw.githubusercontent.com/ashgreat/dataviz-blog/main/Images/therealkiyosaki/twitter-2021-04-16.png</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A13" s="3">
         <v>44332</v>
       </c>
@@ -11405,8 +11620,15 @@
       <c r="C13" s="3">
         <v>44333</v>
       </c>
-    </row>
-    <row r="14" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="D13" t="s">
+        <v>20</v>
+      </c>
+      <c r="E13" t="str">
+        <f t="shared" si="0"/>
+        <v>https://raw.githubusercontent.com/ashgreat/dataviz-blog/main/Images/therealkiyosaki/twitter-2021-05-16.png</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A14" s="3">
         <v>44365</v>
       </c>
@@ -11417,8 +11639,15 @@
       <c r="C14" s="3">
         <v>44365</v>
       </c>
-    </row>
-    <row r="15" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="D14" t="s">
+        <v>21</v>
+      </c>
+      <c r="E14" t="str">
+        <f t="shared" si="0"/>
+        <v>https://raw.githubusercontent.com/ashgreat/dataviz-blog/main/Images/therealkiyosaki/twitter-2021-06-18.png</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A15" s="3">
         <v>44374</v>
       </c>
@@ -11429,8 +11658,15 @@
       <c r="C15" s="3">
         <v>44375</v>
       </c>
-    </row>
-    <row r="16" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="D15" t="s">
+        <v>22</v>
+      </c>
+      <c r="E15" t="str">
+        <f t="shared" si="0"/>
+        <v>https://raw.githubusercontent.com/ashgreat/dataviz-blog/main/Images/therealkiyosaki/twitter-2021-06-27.png</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A16" s="3">
         <v>44408</v>
       </c>
@@ -11441,8 +11677,15 @@
       <c r="C16" s="3">
         <v>44407</v>
       </c>
-    </row>
-    <row r="17" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="D16" t="s">
+        <v>23</v>
+      </c>
+      <c r="E16" t="str">
+        <f t="shared" si="0"/>
+        <v>https://raw.githubusercontent.com/ashgreat/dataviz-blog/main/Images/therealkiyosaki/twitter-2021-07-31.png</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A17" s="3">
         <v>44461</v>
       </c>
@@ -11453,8 +11696,15 @@
       <c r="C17" s="3">
         <v>44461</v>
       </c>
-    </row>
-    <row r="18" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="D17" t="s">
+        <v>24</v>
+      </c>
+      <c r="E17" t="str">
+        <f t="shared" si="0"/>
+        <v>https://raw.githubusercontent.com/ashgreat/dataviz-blog/main/Images/therealkiyosaki/twitter-2021-09-22.png</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A18" s="3">
         <v>44462</v>
       </c>
@@ -11465,8 +11715,15 @@
       <c r="C18" s="3">
         <v>44462</v>
       </c>
-    </row>
-    <row r="19" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="D18" t="s">
+        <v>25</v>
+      </c>
+      <c r="E18" t="str">
+        <f t="shared" si="0"/>
+        <v>https://raw.githubusercontent.com/ashgreat/dataviz-blog/main/Images/therealkiyosaki/twitter-2021-09-23.png</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A19" s="3">
         <v>44465</v>
       </c>
@@ -11476,6 +11733,197 @@
       </c>
       <c r="C19" s="3">
         <v>44466</v>
+      </c>
+      <c r="D19" t="s">
+        <v>26</v>
+      </c>
+      <c r="E19" t="str">
+        <f t="shared" si="0"/>
+        <v>https://raw.githubusercontent.com/ashgreat/dataviz-blog/main/Images/therealkiyosaki/twitter-2021-09-26.png</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E21" s="10"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{52C6176E-E130-3943-B696-F54A57ACD4DC}">
+  <dimension ref="A1:B20"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B29" sqref="B29"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="11.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="96.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="97.6640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" ht="17" x14ac:dyDescent="0.2">
+      <c r="A2" s="3">
+        <v>43910</v>
+      </c>
+      <c r="B2" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" ht="17" x14ac:dyDescent="0.2">
+      <c r="A3" s="3">
+        <v>43913</v>
+      </c>
+      <c r="B3" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" ht="17" x14ac:dyDescent="0.2">
+      <c r="A4" s="3">
+        <v>43938</v>
+      </c>
+      <c r="B4" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" ht="17" x14ac:dyDescent="0.2">
+      <c r="A5" s="3">
+        <v>44032</v>
+      </c>
+      <c r="B5" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" ht="17" x14ac:dyDescent="0.2">
+      <c r="A6" s="3">
+        <v>44043</v>
+      </c>
+      <c r="B6" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" ht="17" x14ac:dyDescent="0.2">
+      <c r="A7" s="3">
+        <v>44056</v>
+      </c>
+      <c r="B7" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" ht="17" x14ac:dyDescent="0.2">
+      <c r="A8" s="3">
+        <v>44099</v>
+      </c>
+      <c r="B8" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" ht="17" x14ac:dyDescent="0.2">
+      <c r="A9" s="3">
+        <v>44106</v>
+      </c>
+      <c r="B9" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" ht="17" x14ac:dyDescent="0.2">
+      <c r="A10" s="3">
+        <v>44110</v>
+      </c>
+      <c r="B10" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" ht="17" x14ac:dyDescent="0.2">
+      <c r="A11" s="3">
+        <v>44132</v>
+      </c>
+      <c r="B11" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" ht="17" x14ac:dyDescent="0.2">
+      <c r="A12" s="3">
+        <v>44295</v>
+      </c>
+      <c r="B12" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" ht="17" x14ac:dyDescent="0.2">
+      <c r="A13" s="3">
+        <v>44302</v>
+      </c>
+      <c r="B13" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" ht="17" x14ac:dyDescent="0.2">
+      <c r="A14" s="3">
+        <v>44333</v>
+      </c>
+      <c r="B14" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" ht="17" x14ac:dyDescent="0.2">
+      <c r="A15" s="3">
+        <v>44365</v>
+      </c>
+      <c r="B15" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" ht="17" x14ac:dyDescent="0.2">
+      <c r="A16" s="3">
+        <v>44375</v>
+      </c>
+      <c r="B16" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" ht="17" x14ac:dyDescent="0.2">
+      <c r="A17" s="3">
+        <v>44407</v>
+      </c>
+      <c r="B17" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" ht="17" x14ac:dyDescent="0.2">
+      <c r="A18" s="3">
+        <v>44461</v>
+      </c>
+      <c r="B18" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" ht="17" x14ac:dyDescent="0.2">
+      <c r="A19" s="3">
+        <v>44462</v>
+      </c>
+      <c r="B19" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" ht="17" x14ac:dyDescent="0.2">
+      <c r="A20" s="3">
+        <v>44466</v>
+      </c>
+      <c r="B20" t="s">
+        <v>46</v>
       </c>
     </row>
   </sheetData>

</xml_diff>